<commit_message>
mapa salda relativní migrace
</commit_message>
<xml_diff>
--- a/src/ORP-CZSO.xlsx
+++ b/src/ORP-CZSO.xlsx
@@ -1580,10 +1580,10 @@
     <t>vek</t>
   </si>
   <si>
-    <t>zastavenost</t>
-  </si>
-  <si>
     <t>pristehovanost</t>
+  </si>
+  <si>
+    <t>rel_migrace</t>
   </si>
 </sst>
 </file>
@@ -2265,8 +2265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2291,7 +2291,7 @@
         <v>513</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E1" s="30" t="s">
         <v>514</v>
@@ -2306,7 +2306,7 @@
         <v>517</v>
       </c>
       <c r="I1" s="30" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2343,8 +2343,8 @@
         <v>41.649161964100003</v>
       </c>
       <c r="I2" s="30">
-        <f>'uap2016'!X7</f>
-        <v>9.3028176713817547</v>
+        <f>'uap2016'!E7/'uap2016'!C7</f>
+        <v>5.407226480249305E-3</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2381,8 +2381,8 @@
         <v>40.546603987700003</v>
       </c>
       <c r="I3" s="30">
-        <f>'uap2016'!X8</f>
-        <v>11.68299998726379</v>
+        <f>'uap2016'!E8/'uap2016'!C8</f>
+        <v>1.2027881342194846E-2</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2419,8 +2419,8 @@
         <v>38.339977967300001</v>
       </c>
       <c r="I4" s="30">
-        <f>'uap2016'!X9</f>
-        <v>14.176525536616955</v>
+        <f>'uap2016'!E9/'uap2016'!C9</f>
+        <v>1.9449562194913485E-2</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2457,8 +2457,8 @@
         <v>42.459357910100003</v>
       </c>
       <c r="I5" s="30">
-        <f>'uap2016'!X10</f>
-        <v>10.243667532737966</v>
+        <f>'uap2016'!E10/'uap2016'!C10</f>
+        <v>3.6983121532832355E-3</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2495,8 +2495,8 @@
         <v>38.777972726199998</v>
       </c>
       <c r="I6" s="30">
-        <f>'uap2016'!X11</f>
-        <v>12.647505616122301</v>
+        <f>'uap2016'!E11/'uap2016'!C11</f>
+        <v>1.4364372931644415E-2</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2533,8 +2533,8 @@
         <v>40.0446926021</v>
       </c>
       <c r="I7" s="30">
-        <f>'uap2016'!X12</f>
-        <v>10.546105579740676</v>
+        <f>'uap2016'!E12/'uap2016'!C12</f>
+        <v>1.0949081924325373E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2571,8 +2571,8 @@
         <v>41.140674629800003</v>
       </c>
       <c r="I8" s="30">
-        <f>'uap2016'!X13</f>
-        <v>6.8904369177181275</v>
+        <f>'uap2016'!E13/'uap2016'!C13</f>
+        <v>7.64997986847403E-3</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2609,8 +2609,8 @@
         <v>42.211848341200003</v>
       </c>
       <c r="I9" s="30">
-        <f>'uap2016'!X14</f>
-        <v>9.8378191690614152</v>
+        <f>'uap2016'!E14/'uap2016'!C14</f>
+        <v>6.4996614759647931E-3</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2647,8 +2647,8 @@
         <v>41.6172295187</v>
       </c>
       <c r="I10" s="30">
-        <f>'uap2016'!X15</f>
-        <v>15.292278305201442</v>
+        <f>'uap2016'!E15/'uap2016'!C15</f>
+        <v>5.6704334352767477E-3</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2685,8 +2685,8 @@
         <v>42.120312365399997</v>
       </c>
       <c r="I11" s="30">
-        <f>'uap2016'!X16</f>
-        <v>11.014616727482354</v>
+        <f>'uap2016'!E16/'uap2016'!C16</f>
+        <v>6.436843854229486E-3</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -2723,8 +2723,8 @@
         <v>40.993803104800001</v>
       </c>
       <c r="I12" s="30">
-        <f>'uap2016'!X17</f>
-        <v>19.796281295130104</v>
+        <f>'uap2016'!E17/'uap2016'!C17</f>
+        <v>1.0285568261675078E-2</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -2761,8 +2761,8 @@
         <v>42.996408279199997</v>
       </c>
       <c r="I13" s="30">
-        <f>'uap2016'!X18</f>
-        <v>8.9162815381307734</v>
+        <f>'uap2016'!E18/'uap2016'!C18</f>
+        <v>2.9626623376623378E-3</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -2799,8 +2799,8 @@
         <v>37.070932069500003</v>
       </c>
       <c r="I14" s="30">
-        <f>'uap2016'!X19</f>
-        <v>20.08514895326595</v>
+        <f>'uap2016'!E19/'uap2016'!C19</f>
+        <v>1.6706161137440757E-2</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -2837,8 +2837,8 @@
         <v>41.565602714900002</v>
       </c>
       <c r="I15" s="30">
-        <f>'uap2016'!X20</f>
-        <v>11.213202933386942</v>
+        <f>'uap2016'!E20/'uap2016'!C20</f>
+        <v>4.4713489715897366E-3</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2875,8 +2875,8 @@
         <v>41.236855561799999</v>
       </c>
       <c r="I16" s="30">
-        <f>'uap2016'!X21</f>
-        <v>10.455280132278347</v>
+        <f>'uap2016'!E21/'uap2016'!C21</f>
+        <v>1.2783753675329182E-3</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -2913,8 +2913,8 @@
         <v>41.672375945900001</v>
       </c>
       <c r="I17" s="30">
-        <f>'uap2016'!X22</f>
-        <v>8.1639636737897003</v>
+        <f>'uap2016'!E22/'uap2016'!C22</f>
+        <v>1.1264513892900467E-2</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -2951,8 +2951,8 @@
         <v>40.796528371199997</v>
       </c>
       <c r="I18" s="30">
-        <f>'uap2016'!X23</f>
-        <v>14.448450685155539</v>
+        <f>'uap2016'!E23/'uap2016'!C23</f>
+        <v>7.7534099180353805E-3</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -2989,8 +2989,8 @@
         <v>42.009819801600003</v>
       </c>
       <c r="I19" s="30">
-        <f>'uap2016'!X24</f>
-        <v>9.6192714168156925</v>
+        <f>'uap2016'!E24/'uap2016'!C24</f>
+        <v>1.0123506782749544E-3</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -3027,8 +3027,8 @@
         <v>43.132910981199998</v>
       </c>
       <c r="I20" s="30">
-        <f>'uap2016'!X25</f>
-        <v>9.2051329064587737</v>
+        <f>'uap2016'!E25/'uap2016'!C25</f>
+        <v>1.267056530214425E-3</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -3065,8 +3065,8 @@
         <v>42.706625531500002</v>
       </c>
       <c r="I21" s="30">
-        <f>'uap2016'!X26</f>
-        <v>10.043369802627385</v>
+        <f>'uap2016'!E26/'uap2016'!C26</f>
+        <v>-8.0170648952770896E-4</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -3103,8 +3103,8 @@
         <v>42.348686470600001</v>
       </c>
       <c r="I22" s="30">
-        <f>'uap2016'!X27</f>
-        <v>7.9887463819168101</v>
+        <f>'uap2016'!E27/'uap2016'!C27</f>
+        <v>1.3560180079191452E-3</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -3141,8 +3141,8 @@
         <v>38.768539089699999</v>
       </c>
       <c r="I23" s="30">
-        <f>'uap2016'!X28</f>
-        <v>10.614020348586992</v>
+        <f>'uap2016'!E28/'uap2016'!C28</f>
+        <v>1.786357631800168E-2</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -3179,8 +3179,8 @@
         <v>42.760822166700002</v>
       </c>
       <c r="I24" s="30">
-        <f>'uap2016'!X29</f>
-        <v>9.5040676702494977</v>
+        <f>'uap2016'!E29/'uap2016'!C29</f>
+        <v>5.4508289802407449E-4</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -3217,8 +3217,8 @@
         <v>41.410861761699998</v>
       </c>
       <c r="I25" s="30">
-        <f>'uap2016'!X30</f>
-        <v>9.819127217182281</v>
+        <f>'uap2016'!E30/'uap2016'!C30</f>
+        <v>2.0081833471395939E-4</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -3255,8 +3255,8 @@
         <v>42.9855421687</v>
       </c>
       <c r="I26" s="30">
-        <f>'uap2016'!X31</f>
-        <v>7.5574524638918898</v>
+        <f>'uap2016'!E31/'uap2016'!C31</f>
+        <v>8.5503303536727557E-4</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -3293,8 +3293,8 @@
         <v>42.482034474400002</v>
       </c>
       <c r="I27" s="30">
-        <f>'uap2016'!X32</f>
-        <v>7.397799465735341</v>
+        <f>'uap2016'!E32/'uap2016'!C32</f>
+        <v>3.7225863882819456E-3</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -3331,8 +3331,8 @@
         <v>43.343594981000003</v>
       </c>
       <c r="I28" s="30">
-        <f>'uap2016'!X33</f>
-        <v>8.6652204598847966</v>
+        <f>'uap2016'!E33/'uap2016'!C33</f>
+        <v>-2.6262036766851473E-3</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -3369,8 +3369,8 @@
         <v>41.806222322899998</v>
       </c>
       <c r="I29" s="30">
-        <f>'uap2016'!X34</f>
-        <v>10.794151679817695</v>
+        <f>'uap2016'!E34/'uap2016'!C34</f>
+        <v>4.7491445249597426E-3</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -3407,8 +3407,8 @@
         <v>41.146398233900001</v>
       </c>
       <c r="I30" s="30">
-        <f>'uap2016'!X35</f>
-        <v>13.758290453440502</v>
+        <f>'uap2016'!E35/'uap2016'!C35</f>
+        <v>-1.5117339348274703E-3</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -3445,8 +3445,8 @@
         <v>42.787593000100003</v>
       </c>
       <c r="I31" s="30">
-        <f>'uap2016'!X36</f>
-        <v>7.20861766270444</v>
+        <f>'uap2016'!E36/'uap2016'!C36</f>
+        <v>-6.8636697055433306E-3</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -3483,8 +3483,8 @@
         <v>42.598365860900003</v>
       </c>
       <c r="I32" s="30">
-        <f>'uap2016'!X37</f>
-        <v>7.9298865169354933</v>
+        <f>'uap2016'!E37/'uap2016'!C37</f>
+        <v>-2.6882858473392321E-3</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -3521,8 +3521,8 @@
         <v>40.709948154599999</v>
       </c>
       <c r="I33" s="30">
-        <f>'uap2016'!X38</f>
-        <v>8.2568571587937409</v>
+        <f>'uap2016'!E38/'uap2016'!C38</f>
+        <v>2.001950618551409E-3</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -3559,8 +3559,8 @@
         <v>44.398141588100003</v>
       </c>
       <c r="I34" s="30">
-        <f>'uap2016'!X39</f>
-        <v>6.9633987270700857</v>
+        <f>'uap2016'!E39/'uap2016'!C39</f>
+        <v>-3.2699329663741891E-3</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -3597,8 +3597,8 @@
         <v>42.728956036600003</v>
       </c>
       <c r="I35" s="30">
-        <f>'uap2016'!X40</f>
-        <v>7.7646355796705535</v>
+        <f>'uap2016'!E40/'uap2016'!C40</f>
+        <v>3.8080006092800975E-3</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -3635,8 +3635,8 @@
         <v>41.672920359300001</v>
       </c>
       <c r="I36" s="30">
-        <f>'uap2016'!X41</f>
-        <v>10.537849587027329</v>
+        <f>'uap2016'!E41/'uap2016'!C41</f>
+        <v>-2.4033406434944573E-3</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -3673,8 +3673,8 @@
         <v>43.461759082199997</v>
       </c>
       <c r="I37" s="30">
-        <f>'uap2016'!X42</f>
-        <v>8.7399699307918493</v>
+        <f>'uap2016'!E42/'uap2016'!C42</f>
+        <v>1.3202221615223528E-3</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -3711,8 +3711,8 @@
         <v>42.552638551599998</v>
       </c>
       <c r="I38" s="30">
-        <f>'uap2016'!X43</f>
-        <v>9.5193463838738648</v>
+        <f>'uap2016'!E43/'uap2016'!C43</f>
+        <v>3.9743872819606975E-4</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -3749,8 +3749,8 @@
         <v>42.830515753999997</v>
       </c>
       <c r="I39" s="30">
-        <f>'uap2016'!X44</f>
-        <v>8.5007458585504576</v>
+        <f>'uap2016'!E44/'uap2016'!C44</f>
+        <v>-5.35298584570952E-4</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -3787,8 +3787,8 @@
         <v>41.427931747099997</v>
       </c>
       <c r="I40" s="30">
-        <f>'uap2016'!X45</f>
-        <v>6.6607410439342054</v>
+        <f>'uap2016'!E45/'uap2016'!C45</f>
+        <v>1.5897408722378252E-3</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -3825,8 +3825,8 @@
         <v>43.251260233099998</v>
       </c>
       <c r="I41" s="30">
-        <f>'uap2016'!X46</f>
-        <v>7.7675626625595555</v>
+        <f>'uap2016'!E46/'uap2016'!C46</f>
+        <v>1.9357180304069041E-3</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -3863,8 +3863,8 @@
         <v>41.288338771500001</v>
       </c>
       <c r="I42" s="30">
-        <f>'uap2016'!X47</f>
-        <v>8.5146904758896866</v>
+        <f>'uap2016'!E47/'uap2016'!C47</f>
+        <v>-5.6745637679103417E-4</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -3901,8 +3901,8 @@
         <v>42.478515625</v>
       </c>
       <c r="I43" s="30">
-        <f>'uap2016'!X48</f>
-        <v>9.9579169952720274</v>
+        <f>'uap2016'!E48/'uap2016'!C48</f>
+        <v>5.744485294117647E-5</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -3939,8 +3939,8 @@
         <v>41.797119411899999</v>
       </c>
       <c r="I44" s="30">
-        <f>'uap2016'!X49</f>
-        <v>8.9042474835014271</v>
+        <f>'uap2016'!E49/'uap2016'!C49</f>
+        <v>6.1543721685614157E-3</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -3977,8 +3977,8 @@
         <v>42.619522577399998</v>
       </c>
       <c r="I45" s="30">
-        <f>'uap2016'!X50</f>
-        <v>8.0112206555573682</v>
+        <f>'uap2016'!E50/'uap2016'!C50</f>
+        <v>3.171688506802437E-3</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -4015,8 +4015,8 @@
         <v>42.250388975299998</v>
       </c>
       <c r="I46" s="30">
-        <f>'uap2016'!X51</f>
-        <v>7.4141257467956203</v>
+        <f>'uap2016'!E51/'uap2016'!C51</f>
+        <v>9.8787384850954532E-5</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -4053,8 +4053,8 @@
         <v>43.924879807700002</v>
       </c>
       <c r="I47" s="30">
-        <f>'uap2016'!X52</f>
-        <v>9.9590773032004858</v>
+        <f>'uap2016'!E52/'uap2016'!C52</f>
+        <v>-2.0604395604395605E-3</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -4091,8 +4091,8 @@
         <v>41.607865322599999</v>
       </c>
       <c r="I48" s="30">
-        <f>'uap2016'!X53</f>
-        <v>8.0995356795179454</v>
+        <f>'uap2016'!E53/'uap2016'!C53</f>
+        <v>9.4630734416786665E-3</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -4129,8 +4129,8 @@
         <v>42.767506087800001</v>
       </c>
       <c r="I49" s="30">
-        <f>'uap2016'!X54</f>
-        <v>8.6046659239459817</v>
+        <f>'uap2016'!E54/'uap2016'!C54</f>
+        <v>-3.9595335669458136E-4</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -4167,8 +4167,8 @@
         <v>42.919053605099997</v>
       </c>
       <c r="I50" s="30">
-        <f>'uap2016'!X55</f>
-        <v>6.8417580280957573</v>
+        <f>'uap2016'!E55/'uap2016'!C55</f>
+        <v>5.9710873664362034E-3</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -4205,8 +4205,8 @@
         <v>43.964587507600001</v>
       </c>
       <c r="I51" s="30">
-        <f>'uap2016'!X56</f>
-        <v>7.7044897578094957</v>
+        <f>'uap2016'!E56/'uap2016'!C56</f>
+        <v>-2.9619304817492813E-3</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -4243,8 +4243,8 @@
         <v>40.979069850899997</v>
       </c>
       <c r="I52" s="30">
-        <f>'uap2016'!X57</f>
-        <v>9.0233559932627276</v>
+        <f>'uap2016'!E57/'uap2016'!C57</f>
+        <v>7.1591337268763567E-3</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -4281,8 +4281,8 @@
         <v>42.9419582194</v>
       </c>
       <c r="I53" s="30">
-        <f>'uap2016'!X58</f>
-        <v>24.87048254201385</v>
+        <f>'uap2016'!E58/'uap2016'!C58</f>
+        <v>5.0969962618502519E-3</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -4319,8 +4319,8 @@
         <v>42.247390583700003</v>
       </c>
       <c r="I54" s="30">
-        <f>'uap2016'!X59</f>
-        <v>8.2029362888154083</v>
+        <f>'uap2016'!E59/'uap2016'!C59</f>
+        <v>6.6299332526990103E-3</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -4357,8 +4357,8 @@
         <v>42.640523825300001</v>
       </c>
       <c r="I55" s="30">
-        <f>'uap2016'!X60</f>
-        <v>9.0558919185388334</v>
+        <f>'uap2016'!E60/'uap2016'!C60</f>
+        <v>5.9148264984227126E-3</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -4395,8 +4395,8 @@
         <v>41.542708650500003</v>
       </c>
       <c r="I56" s="30">
-        <f>'uap2016'!X61</f>
-        <v>10.009455041709181</v>
+        <f>'uap2016'!E61/'uap2016'!C61</f>
+        <v>3.0009133214456574E-3</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -4433,8 +4433,8 @@
         <v>41.887967787800001</v>
       </c>
       <c r="I57" s="30">
-        <f>'uap2016'!X62</f>
-        <v>7.6685200348847697</v>
+        <f>'uap2016'!E62/'uap2016'!C62</f>
+        <v>4.7370914258645192E-4</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -4471,8 +4471,8 @@
         <v>43.807249001800002</v>
       </c>
       <c r="I58" s="30">
-        <f>'uap2016'!X63</f>
-        <v>8.8791515803011123</v>
+        <f>'uap2016'!E63/'uap2016'!C63</f>
+        <v>4.1164121351829743E-5</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -4509,8 +4509,8 @@
         <v>41.041296342400003</v>
       </c>
       <c r="I59" s="30">
-        <f>'uap2016'!X64</f>
-        <v>6.821950077994102</v>
+        <f>'uap2016'!E64/'uap2016'!C64</f>
+        <v>2.7134036603261623E-3</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -4547,8 +4547,8 @@
         <v>41.052012664000003</v>
       </c>
       <c r="I60" s="30">
-        <f>'uap2016'!X65</f>
-        <v>11.148075738503978</v>
+        <f>'uap2016'!E65/'uap2016'!C65</f>
+        <v>1.7526006331976482E-3</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -4585,8 +4585,8 @@
         <v>41.854868297700001</v>
       </c>
       <c r="I61" s="30">
-        <f>'uap2016'!X66</f>
-        <v>11.209131113600298</v>
+        <f>'uap2016'!E66/'uap2016'!C66</f>
+        <v>1.3359653845386931E-3</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -4623,8 +4623,8 @@
         <v>43.540142027000002</v>
       </c>
       <c r="I62" s="30">
-        <f>'uap2016'!X67</f>
-        <v>22.631247345977997</v>
+        <f>'uap2016'!E67/'uap2016'!C67</f>
+        <v>-1.5755403075728687E-3</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -4661,8 +4661,8 @@
         <v>42.608674353799998</v>
       </c>
       <c r="I63" s="30">
-        <f>'uap2016'!X68</f>
-        <v>6.610076706477817</v>
+        <f>'uap2016'!E68/'uap2016'!C68</f>
+        <v>-8.6668173939256909E-3</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -4699,8 +4699,8 @@
         <v>43.640970080800003</v>
       </c>
       <c r="I64" s="30">
-        <f>'uap2016'!X69</f>
-        <v>7.9373643798694173</v>
+        <f>'uap2016'!E69/'uap2016'!C69</f>
+        <v>-6.2505208767397286E-4</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -4737,8 +4737,8 @@
         <v>42.031990353200001</v>
       </c>
       <c r="I65" s="30">
-        <f>'uap2016'!X70</f>
-        <v>12.006393020172425</v>
+        <f>'uap2016'!E70/'uap2016'!C70</f>
+        <v>-9.0083699815576672E-3</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -4775,8 +4775,8 @@
         <v>41.543686888700002</v>
       </c>
       <c r="I66" s="30">
-        <f>'uap2016'!X71</f>
-        <v>26.866870643324038</v>
+        <f>'uap2016'!E71/'uap2016'!C71</f>
+        <v>-3.6779245432255001E-3</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -4813,8 +4813,8 @@
         <v>40.780670628899998</v>
       </c>
       <c r="I67" s="30">
-        <f>'uap2016'!X72</f>
-        <v>36.593596176521501</v>
+        <f>'uap2016'!E72/'uap2016'!C72</f>
+        <v>6.7417723764747629E-3</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -4851,8 +4851,8 @@
         <v>41.997613073399997</v>
       </c>
       <c r="I68" s="30">
-        <f>'uap2016'!X73</f>
-        <v>9.0404272323916679</v>
+        <f>'uap2016'!E73/'uap2016'!C73</f>
+        <v>-1.3896931094383323E-3</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -4889,8 +4889,8 @@
         <v>41.0415210273</v>
       </c>
       <c r="I69" s="30">
-        <f>'uap2016'!X74</f>
-        <v>20.242206931794733</v>
+        <f>'uap2016'!E74/'uap2016'!C74</f>
+        <v>-4.6604608950537795E-4</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -4927,8 +4927,8 @@
         <v>41.358564337899999</v>
       </c>
       <c r="I70" s="30">
-        <f>'uap2016'!X75</f>
-        <v>13.18502964631926</v>
+        <f>'uap2016'!E75/'uap2016'!C75</f>
+        <v>-8.1944184304176809E-4</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -4965,8 +4965,8 @@
         <v>41.603695076000001</v>
       </c>
       <c r="I71" s="30">
-        <f>'uap2016'!X76</f>
-        <v>11.123206268790113</v>
+        <f>'uap2016'!E76/'uap2016'!C76</f>
+        <v>2.0256241454398136E-3</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -5003,8 +5003,8 @@
         <v>42.478418223399999</v>
       </c>
       <c r="I72" s="30">
-        <f>'uap2016'!X77</f>
-        <v>25.578214025532674</v>
+        <f>'uap2016'!E77/'uap2016'!C77</f>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -5041,8 +5041,8 @@
         <v>41.592475443399998</v>
       </c>
       <c r="I73" s="30">
-        <f>'uap2016'!X78</f>
-        <v>11.436682888203654</v>
+        <f>'uap2016'!E78/'uap2016'!C78</f>
+        <v>1.6792804398334522E-3</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -5079,8 +5079,8 @@
         <v>42.613952134999998</v>
       </c>
       <c r="I74" s="30">
-        <f>'uap2016'!X79</f>
-        <v>10.957684222313318</v>
+        <f>'uap2016'!E79/'uap2016'!C79</f>
+        <v>4.6919327853349822E-3</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -5117,8 +5117,8 @@
         <v>41.240568104899999</v>
       </c>
       <c r="I75" s="30">
-        <f>'uap2016'!X80</f>
-        <v>44.28830896361363</v>
+        <f>'uap2016'!E80/'uap2016'!C80</f>
+        <v>-3.9573456568795396E-3</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -5155,8 +5155,8 @@
         <v>41.808773938999998</v>
       </c>
       <c r="I76" s="30">
-        <f>'uap2016'!X81</f>
-        <v>11.313152967389087</v>
+        <f>'uap2016'!E81/'uap2016'!C81</f>
+        <v>4.5174015397340455E-3</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -5193,8 +5193,8 @@
         <v>41.785122826399999</v>
       </c>
       <c r="I77" s="30">
-        <f>'uap2016'!X82</f>
-        <v>9.9297064095605521</v>
+        <f>'uap2016'!E82/'uap2016'!C82</f>
+        <v>3.9562057226975806E-3</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -5231,8 +5231,8 @@
         <v>41.553705334100002</v>
       </c>
       <c r="I78" s="30">
-        <f>'uap2016'!X83</f>
-        <v>8.4682785829810836</v>
+        <f>'uap2016'!E83/'uap2016'!C83</f>
+        <v>-3.7038161449952944E-3</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -5269,8 +5269,8 @@
         <v>41.931822901899999</v>
       </c>
       <c r="I79" s="30">
-        <f>'uap2016'!X84</f>
-        <v>20.949497735104337</v>
+        <f>'uap2016'!E84/'uap2016'!C84</f>
+        <v>-2.105163787406778E-3</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -5307,8 +5307,8 @@
         <v>41.4774678112</v>
       </c>
       <c r="I80" s="30">
-        <f>'uap2016'!X85</f>
-        <v>20.622632762115241</v>
+        <f>'uap2016'!E85/'uap2016'!C85</f>
+        <v>-2.7829935622317595E-3</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -5345,8 +5345,8 @@
         <v>41.844856702900003</v>
       </c>
       <c r="I81" s="30">
-        <f>'uap2016'!X86</f>
-        <v>12.088053499865717</v>
+        <f>'uap2016'!E86/'uap2016'!C86</f>
+        <v>-4.9669696518154271E-3</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -5383,8 +5383,8 @@
         <v>41.2925104941</v>
       </c>
       <c r="I82" s="30">
-        <f>'uap2016'!X87</f>
-        <v>14.14619553481193</v>
+        <f>'uap2016'!E87/'uap2016'!C87</f>
+        <v>-3.5348700198836441E-3</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -5421,8 +5421,8 @@
         <v>40.7226671536</v>
       </c>
       <c r="I83" s="30">
-        <f>'uap2016'!X88</f>
-        <v>11.036385050802402</v>
+        <f>'uap2016'!E88/'uap2016'!C88</f>
+        <v>-1.6565361437925548E-3</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -5459,8 +5459,8 @@
         <v>41.256849454899999</v>
       </c>
       <c r="I84" s="30">
-        <f>'uap2016'!X89</f>
-        <v>6.1212738980444525</v>
+        <f>'uap2016'!E89/'uap2016'!C89</f>
+        <v>-1.3882650769670491E-3</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -5497,8 +5497,8 @@
         <v>41.7505566329</v>
       </c>
       <c r="I85" s="30">
-        <f>'uap2016'!X90</f>
-        <v>14.016022346709459</v>
+        <f>'uap2016'!E90/'uap2016'!C90</f>
+        <v>3.7527831645478705E-3</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -5535,8 +5535,8 @@
         <v>42.6483879671</v>
       </c>
       <c r="I86" s="30">
-        <f>'uap2016'!X91</f>
-        <v>6.9202520209328018</v>
+        <f>'uap2016'!E91/'uap2016'!C91</f>
+        <v>-1.3040154683214174E-3</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -5573,8 +5573,8 @@
         <v>41.425232343600001</v>
       </c>
       <c r="I87" s="30">
-        <f>'uap2016'!X92</f>
-        <v>11.204677394620402</v>
+        <f>'uap2016'!E92/'uap2016'!C92</f>
+        <v>3.0352605381322008E-3</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -5611,8 +5611,8 @@
         <v>42.6133832529</v>
       </c>
       <c r="I88" s="30">
-        <f>'uap2016'!X93</f>
-        <v>9.5778893284656466</v>
+        <f>'uap2016'!E93/'uap2016'!C93</f>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -5649,8 +5649,8 @@
         <v>42.836020151100001</v>
       </c>
       <c r="I89" s="30">
-        <f>'uap2016'!X94</f>
-        <v>9.8234391522681488</v>
+        <f>'uap2016'!E94/'uap2016'!C94</f>
+        <v>2.4413873280372022E-3</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -5687,8 +5687,8 @@
         <v>42.931731095700002</v>
       </c>
       <c r="I90" s="30">
-        <f>'uap2016'!X95</f>
-        <v>7.2288866745205098</v>
+        <f>'uap2016'!E95/'uap2016'!C95</f>
+        <v>-9.5067177571906674E-3</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -5725,8 +5725,8 @@
         <v>42.6664245945</v>
       </c>
       <c r="I91" s="30">
-        <f>'uap2016'!X96</f>
-        <v>10.226415787292424</v>
+        <f>'uap2016'!E96/'uap2016'!C96</f>
+        <v>2.2089082546598885E-3</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -5763,8 +5763,8 @@
         <v>43.017898383400002</v>
       </c>
       <c r="I92" s="30">
-        <f>'uap2016'!X97</f>
-        <v>12.251482901535315</v>
+        <f>'uap2016'!E97/'uap2016'!C97</f>
+        <v>2.2269877928076543E-3</v>
       </c>
     </row>
     <row r="93" spans="1:9">
@@ -5801,8 +5801,8 @@
         <v>42.610427938999997</v>
       </c>
       <c r="I93" s="30">
-        <f>'uap2016'!X98</f>
-        <v>7.0102744565086432</v>
+        <f>'uap2016'!E98/'uap2016'!C98</f>
+        <v>-8.0545991146089516E-3</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -5839,8 +5839,8 @@
         <v>42.2040765721</v>
       </c>
       <c r="I94" s="30">
-        <f>'uap2016'!X99</f>
-        <v>7.7289839793387713</v>
+        <f>'uap2016'!E99/'uap2016'!C99</f>
+        <v>-8.4308668914897839E-4</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -5877,8 +5877,8 @@
         <v>43.413421828899999</v>
       </c>
       <c r="I95" s="30">
-        <f>'uap2016'!X100</f>
-        <v>8.6379038188260573</v>
+        <f>'uap2016'!E100/'uap2016'!C100</f>
+        <v>-2.3230088495575221E-3</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -5915,8 +5915,8 @@
         <v>42.681170068</v>
       </c>
       <c r="I96" s="30">
-        <f>'uap2016'!X101</f>
-        <v>8.8541848652653723</v>
+        <f>'uap2016'!E101/'uap2016'!C101</f>
+        <v>1.0340136054421769E-3</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -5953,8 +5953,8 @@
         <v>43.025769731899999</v>
       </c>
       <c r="I97" s="30">
-        <f>'uap2016'!X102</f>
-        <v>12.43462164058597</v>
+        <f>'uap2016'!E102/'uap2016'!C102</f>
+        <v>9.2573544538160878E-4</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -5991,8 +5991,8 @@
         <v>41.3612824633</v>
       </c>
       <c r="I98" s="30">
-        <f>'uap2016'!X103</f>
-        <v>10.473747921249268</v>
+        <f>'uap2016'!E103/'uap2016'!C103</f>
+        <v>-2.902908091856306E-3</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -6029,8 +6029,8 @@
         <v>42.4921927328</v>
       </c>
       <c r="I99" s="30">
-        <f>'uap2016'!X104</f>
-        <v>8.3961496628749774</v>
+        <f>'uap2016'!E104/'uap2016'!C104</f>
+        <v>1.6744809109176155E-4</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -6067,8 +6067,8 @@
         <v>42.602176541699997</v>
       </c>
       <c r="I100" s="30">
-        <f>'uap2016'!X105</f>
-        <v>8.6603897164254899</v>
+        <f>'uap2016'!E105/'uap2016'!C105</f>
+        <v>-1.1285771866182991E-3</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -6105,8 +6105,8 @@
         <v>42.9955758045</v>
       </c>
       <c r="I101" s="30">
-        <f>'uap2016'!X106</f>
-        <v>9.6876238572020696</v>
+        <f>'uap2016'!E106/'uap2016'!C106</f>
+        <v>-2.2079783815848013E-3</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -6143,8 +6143,8 @@
         <v>43.311872283</v>
       </c>
       <c r="I102" s="30">
-        <f>'uap2016'!X107</f>
-        <v>10.311905657536357</v>
+        <f>'uap2016'!E107/'uap2016'!C107</f>
+        <v>-3.7475640833458252E-4</v>
       </c>
     </row>
     <row r="103" spans="1:9">
@@ -6181,8 +6181,8 @@
         <v>43.312246041800002</v>
       </c>
       <c r="I103" s="30">
-        <f>'uap2016'!X108</f>
-        <v>10.152395002169003</v>
+        <f>'uap2016'!E108/'uap2016'!C108</f>
+        <v>-1.8214936247723133E-3</v>
       </c>
     </row>
     <row r="104" spans="1:9">
@@ -6219,8 +6219,8 @@
         <v>42.675182063199998</v>
       </c>
       <c r="I104" s="30">
-        <f>'uap2016'!X109</f>
-        <v>7.7576396986463738</v>
+        <f>'uap2016'!E109/'uap2016'!C109</f>
+        <v>-3.4979069900797064E-3</v>
       </c>
     </row>
     <row r="105" spans="1:9">
@@ -6257,8 +6257,8 @@
         <v>41.8287472632</v>
       </c>
       <c r="I105" s="30">
-        <f>'uap2016'!X110</f>
-        <v>7.1254829753621447</v>
+        <f>'uap2016'!E110/'uap2016'!C110</f>
+        <v>-2.3965915142907866E-3</v>
       </c>
     </row>
     <row r="106" spans="1:9">
@@ -6295,8 +6295,8 @@
         <v>42.595552875199999</v>
       </c>
       <c r="I106" s="30">
-        <f>'uap2016'!X111</f>
-        <v>9.1818825447384533</v>
+        <f>'uap2016'!E111/'uap2016'!C111</f>
+        <v>-1.8327354751797491E-3</v>
       </c>
     </row>
     <row r="107" spans="1:9">
@@ -6333,8 +6333,8 @@
         <v>42.3063541179</v>
       </c>
       <c r="I107" s="30">
-        <f>'uap2016'!X112</f>
-        <v>8.4222845490478822</v>
+        <f>'uap2016'!E112/'uap2016'!C112</f>
+        <v>1.7990141402511424E-4</v>
       </c>
     </row>
     <row r="108" spans="1:9">
@@ -6371,8 +6371,8 @@
         <v>42.544523744199999</v>
       </c>
       <c r="I108" s="30">
-        <f>'uap2016'!X113</f>
-        <v>12.469624991405949</v>
+        <f>'uap2016'!E113/'uap2016'!C113</f>
+        <v>-5.0507823222618719E-3</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -6409,8 +6409,8 @@
         <v>42.6733472644</v>
       </c>
       <c r="I109" s="30">
-        <f>'uap2016'!X114</f>
-        <v>8.4141448538570156</v>
+        <f>'uap2016'!E114/'uap2016'!C114</f>
+        <v>-1.1398176291793312E-3</v>
       </c>
     </row>
     <row r="110" spans="1:9">
@@ -6447,8 +6447,8 @@
         <v>41.4844222539</v>
       </c>
       <c r="I110" s="30">
-        <f>'uap2016'!X115</f>
-        <v>5.8258904920388863</v>
+        <f>'uap2016'!E115/'uap2016'!C115</f>
+        <v>1.369472182596291E-3</v>
       </c>
     </row>
     <row r="111" spans="1:9">
@@ -6485,8 +6485,8 @@
         <v>42.201563046099999</v>
       </c>
       <c r="I111" s="30">
-        <f>'uap2016'!X116</f>
-        <v>9.0542360187991022</v>
+        <f>'uap2016'!E116/'uap2016'!C116</f>
+        <v>1.5787126863423275E-3</v>
       </c>
     </row>
     <row r="112" spans="1:9">
@@ -6523,8 +6523,8 @@
         <v>42.310598171899997</v>
       </c>
       <c r="I112" s="30">
-        <f>'uap2016'!X117</f>
-        <v>7.2608294212521614</v>
+        <f>'uap2016'!E117/'uap2016'!C117</f>
+        <v>-5.4379266458405642E-3</v>
       </c>
     </row>
     <row r="113" spans="1:9">
@@ -6561,8 +6561,8 @@
         <v>41.262728684800003</v>
       </c>
       <c r="I113" s="30">
-        <f>'uap2016'!X118</f>
-        <v>7.3751259655456538</v>
+        <f>'uap2016'!E118/'uap2016'!C118</f>
+        <v>-3.9264756644804971E-3</v>
       </c>
     </row>
     <row r="114" spans="1:9">
@@ -6599,8 +6599,8 @@
         <v>41.600029949099998</v>
       </c>
       <c r="I114" s="30">
-        <f>'uap2016'!X119</f>
-        <v>7.1979868326411429</v>
+        <f>'uap2016'!E119/'uap2016'!C119</f>
+        <v>1.4600179694519318E-3</v>
       </c>
     </row>
     <row r="115" spans="1:9">
@@ -6637,8 +6637,8 @@
         <v>42.5701121034</v>
       </c>
       <c r="I115" s="30">
-        <f>'uap2016'!X120</f>
-        <v>6.9215002971445214</v>
+        <f>'uap2016'!E120/'uap2016'!C120</f>
+        <v>-1.5200456013680412E-4</v>
       </c>
     </row>
     <row r="116" spans="1:9">
@@ -6675,8 +6675,8 @@
         <v>42.319003572</v>
       </c>
       <c r="I116" s="30">
-        <f>'uap2016'!X121</f>
-        <v>16.973824457656217</v>
+        <f>'uap2016'!E121/'uap2016'!C121</f>
+        <v>4.7653215617152042E-3</v>
       </c>
     </row>
     <row r="117" spans="1:9">
@@ -6713,8 +6713,8 @@
         <v>41.817953964200001</v>
       </c>
       <c r="I117" s="30">
-        <f>'uap2016'!X122</f>
-        <v>7.5333297164986561</v>
+        <f>'uap2016'!E122/'uap2016'!C122</f>
+        <v>-1.5856777493606139E-3</v>
       </c>
     </row>
     <row r="118" spans="1:9">
@@ -6751,8 +6751,8 @@
         <v>42.566321449900002</v>
       </c>
       <c r="I118" s="30">
-        <f>'uap2016'!X123</f>
-        <v>10.722451456405963</v>
+        <f>'uap2016'!E123/'uap2016'!C123</f>
+        <v>8.5241983668591908E-3</v>
       </c>
     </row>
     <row r="119" spans="1:9">
@@ -6789,8 +6789,8 @@
         <v>42.032147266499997</v>
       </c>
       <c r="I119" s="30">
-        <f>'uap2016'!X124</f>
-        <v>8.2818093944669151</v>
+        <f>'uap2016'!E124/'uap2016'!C124</f>
+        <v>-1.4245465193580044E-3</v>
       </c>
     </row>
     <row r="120" spans="1:9">
@@ -6827,8 +6827,8 @@
         <v>42.285600545999998</v>
       </c>
       <c r="I120" s="30">
-        <f>'uap2016'!X125</f>
-        <v>8.2214463738405534</v>
+        <f>'uap2016'!E125/'uap2016'!C125</f>
+        <v>-1.1373976342129209E-4</v>
       </c>
     </row>
     <row r="121" spans="1:9">
@@ -6865,8 +6865,8 @@
         <v>41.9534865806</v>
       </c>
       <c r="I121" s="30">
-        <f>'uap2016'!X126</f>
-        <v>8.511448387210411</v>
+        <f>'uap2016'!E126/'uap2016'!C126</f>
+        <v>-6.4708963732166517E-4</v>
       </c>
     </row>
     <row r="122" spans="1:9">
@@ -6903,8 +6903,8 @@
         <v>41.1841131105</v>
       </c>
       <c r="I122" s="30">
-        <f>'uap2016'!X127</f>
-        <v>7.8642697993308976</v>
+        <f>'uap2016'!E127/'uap2016'!C127</f>
+        <v>-7.5407026563838902E-4</v>
       </c>
     </row>
     <row r="123" spans="1:9">
@@ -6941,8 +6941,8 @@
         <v>42.818779484099998</v>
       </c>
       <c r="I123" s="30">
-        <f>'uap2016'!X128</f>
-        <v>8.1137996779064938</v>
+        <f>'uap2016'!E128/'uap2016'!C128</f>
+        <v>-4.9683830171635048E-3</v>
       </c>
     </row>
     <row r="124" spans="1:9">
@@ -6979,8 +6979,8 @@
         <v>42.1976090283</v>
       </c>
       <c r="I124" s="30">
-        <f>'uap2016'!X129</f>
-        <v>7.9414146963656034</v>
+        <f>'uap2016'!E129/'uap2016'!C129</f>
+        <v>1.9127773527161438E-4</v>
       </c>
     </row>
     <row r="125" spans="1:9">
@@ -7017,8 +7017,8 @@
         <v>43.064329826200002</v>
       </c>
       <c r="I125" s="30">
-        <f>'uap2016'!X130</f>
-        <v>8.0330259212461179</v>
+        <f>'uap2016'!E130/'uap2016'!C130</f>
+        <v>-7.4336688014638608E-4</v>
       </c>
     </row>
     <row r="126" spans="1:9">
@@ -7055,8 +7055,8 @@
         <v>42.867664399100001</v>
       </c>
       <c r="I126" s="30">
-        <f>'uap2016'!X131</f>
-        <v>6.8648603255272835</v>
+        <f>'uap2016'!E131/'uap2016'!C131</f>
+        <v>-2.7210884353741495E-3</v>
       </c>
     </row>
     <row r="127" spans="1:9">
@@ -7093,8 +7093,8 @@
         <v>41.746135695600003</v>
       </c>
       <c r="I127" s="30">
-        <f>'uap2016'!X132</f>
-        <v>8.7136642610204511</v>
+        <f>'uap2016'!E132/'uap2016'!C132</f>
+        <v>-1.1197984362814693E-3</v>
       </c>
     </row>
     <row r="128" spans="1:9">
@@ -7131,8 +7131,8 @@
         <v>42.797107047799997</v>
       </c>
       <c r="I128" s="30">
-        <f>'uap2016'!X133</f>
-        <v>6.6185085096873459</v>
+        <f>'uap2016'!E133/'uap2016'!C133</f>
+        <v>-1.244742037943171E-3</v>
       </c>
     </row>
     <row r="129" spans="1:9">
@@ -7169,8 +7169,8 @@
         <v>43.138776428299998</v>
       </c>
       <c r="I129" s="30">
-        <f>'uap2016'!X134</f>
-        <v>9.3750777959512259</v>
+        <f>'uap2016'!E134/'uap2016'!C134</f>
+        <v>1.4994751836857099E-4</v>
       </c>
     </row>
     <row r="130" spans="1:9">
@@ -7207,8 +7207,8 @@
         <v>42.042265907900003</v>
       </c>
       <c r="I130" s="30">
-        <f>'uap2016'!X135</f>
-        <v>7.1948198642974885</v>
+        <f>'uap2016'!E135/'uap2016'!C135</f>
+        <v>-5.690636316606311E-4</v>
       </c>
     </row>
     <row r="131" spans="1:9">
@@ -7245,8 +7245,8 @@
         <v>44.552974563799999</v>
       </c>
       <c r="I131" s="30">
-        <f>'uap2016'!X136</f>
-        <v>7.0887450685135311</v>
+        <f>'uap2016'!E136/'uap2016'!C136</f>
+        <v>-4.2043304603741857E-4</v>
       </c>
     </row>
     <row r="132" spans="1:9">
@@ -7283,8 +7283,8 @@
         <v>43.123479711000002</v>
       </c>
       <c r="I132" s="30">
-        <f>'uap2016'!X137</f>
-        <v>6.9351862549278902</v>
+        <f>'uap2016'!E137/'uap2016'!C137</f>
+        <v>1.1561978877153974E-3</v>
       </c>
     </row>
     <row r="133" spans="1:9">
@@ -7321,8 +7321,8 @@
         <v>43.661189516100002</v>
       </c>
       <c r="I133" s="30">
-        <f>'uap2016'!X138</f>
-        <v>6.6031793658845261</v>
+        <f>'uap2016'!E138/'uap2016'!C138</f>
+        <v>-7.5604838709677417E-4</v>
       </c>
     </row>
     <row r="134" spans="1:9">
@@ -7359,8 +7359,8 @@
         <v>42.609585889599998</v>
       </c>
       <c r="I134" s="30">
-        <f>'uap2016'!X139</f>
-        <v>7.4858178269430349</v>
+        <f>'uap2016'!E139/'uap2016'!C139</f>
+        <v>-4.0644171779141104E-3</v>
       </c>
     </row>
     <row r="135" spans="1:9">
@@ -7397,8 +7397,8 @@
         <v>42.2473038726</v>
       </c>
       <c r="I135" s="30">
-        <f>'uap2016'!X140</f>
-        <v>7.4680034674873736</v>
+        <f>'uap2016'!E140/'uap2016'!C140</f>
+        <v>-3.4526428047723791E-3</v>
       </c>
     </row>
     <row r="136" spans="1:9">
@@ -7435,8 +7435,8 @@
         <v>40.906135480300001</v>
       </c>
       <c r="I136" s="30">
-        <f>'uap2016'!X141</f>
-        <v>8.0907506686103794</v>
+        <f>'uap2016'!E141/'uap2016'!C141</f>
+        <v>-1.6935036091060521E-3</v>
       </c>
     </row>
     <row r="137" spans="1:9">
@@ -7473,8 +7473,8 @@
         <v>42.212283979399999</v>
       </c>
       <c r="I137" s="30">
-        <f>'uap2016'!X142</f>
-        <v>6.6980830383839258</v>
+        <f>'uap2016'!E142/'uap2016'!C142</f>
+        <v>-4.2269967304997668E-3</v>
       </c>
     </row>
     <row r="138" spans="1:9">
@@ -7511,8 +7511,8 @@
         <v>42.344924413699999</v>
       </c>
       <c r="I138" s="30">
-        <f>'uap2016'!X143</f>
-        <v>8.7701005665134275</v>
+        <f>'uap2016'!E143/'uap2016'!C143</f>
+        <v>1.2009042102288782E-3</v>
       </c>
     </row>
     <row r="139" spans="1:9">
@@ -7549,8 +7549,8 @@
         <v>41.979215093800001</v>
       </c>
       <c r="I139" s="30">
-        <f>'uap2016'!X144</f>
-        <v>9.2446317477128765</v>
+        <f>'uap2016'!E144/'uap2016'!C144</f>
+        <v>4.2615837594917093E-4</v>
       </c>
     </row>
     <row r="140" spans="1:9">
@@ -7587,8 +7587,8 @@
         <v>42.783091649399999</v>
       </c>
       <c r="I140" s="30">
-        <f>'uap2016'!X145</f>
-        <v>36.73880472853353</v>
+        <f>'uap2016'!E145/'uap2016'!C145</f>
+        <v>8.4662131951224033E-4</v>
       </c>
     </row>
     <row r="141" spans="1:9">
@@ -7625,8 +7625,8 @@
         <v>42.577548834200002</v>
       </c>
       <c r="I141" s="30">
-        <f>'uap2016'!X146</f>
-        <v>11.501686761860444</v>
+        <f>'uap2016'!E146/'uap2016'!C146</f>
+        <v>-1.4227608255360461E-3</v>
       </c>
     </row>
     <row r="142" spans="1:9">
@@ -7663,8 +7663,8 @@
         <v>42.178323861899997</v>
       </c>
       <c r="I142" s="30">
-        <f>'uap2016'!X147</f>
-        <v>9.3488024167023553</v>
+        <f>'uap2016'!E147/'uap2016'!C147</f>
+        <v>1.5612314994067321E-3</v>
       </c>
     </row>
     <row r="143" spans="1:9">
@@ -7701,8 +7701,8 @@
         <v>42.7198437192</v>
       </c>
       <c r="I143" s="30">
-        <f>'uap2016'!X148</f>
-        <v>12.425742413476867</v>
+        <f>'uap2016'!E148/'uap2016'!C148</f>
+        <v>-2.3310788626961718E-3</v>
       </c>
     </row>
     <row r="144" spans="1:9">
@@ -7739,8 +7739,8 @@
         <v>41.885920366100002</v>
       </c>
       <c r="I144" s="30">
-        <f>'uap2016'!X149</f>
-        <v>11.025740783416596</v>
+        <f>'uap2016'!E149/'uap2016'!C149</f>
+        <v>3.180892324004576E-3</v>
       </c>
     </row>
     <row r="145" spans="1:9">
@@ -7777,8 +7777,8 @@
         <v>41.9228571429</v>
       </c>
       <c r="I145" s="30">
-        <f>'uap2016'!X150</f>
-        <v>10.668057585858724</v>
+        <f>'uap2016'!E150/'uap2016'!C150</f>
+        <v>4.5962732919254661E-3</v>
       </c>
     </row>
     <row r="146" spans="1:9">
@@ -7815,8 +7815,8 @@
         <v>40.384447962000003</v>
       </c>
       <c r="I146" s="30">
-        <f>'uap2016'!X151</f>
-        <v>12.919787264166047</v>
+        <f>'uap2016'!E151/'uap2016'!C151</f>
+        <v>3.2977179791584222E-3</v>
       </c>
     </row>
     <row r="147" spans="1:9">
@@ -7853,8 +7853,8 @@
         <v>42.804633016799997</v>
       </c>
       <c r="I147" s="30">
-        <f>'uap2016'!X152</f>
-        <v>9.4980655903631348</v>
+        <f>'uap2016'!E152/'uap2016'!C152</f>
+        <v>2.8832465355990846E-4</v>
       </c>
     </row>
     <row r="148" spans="1:9">
@@ -7891,8 +7891,8 @@
         <v>42.0493198992</v>
       </c>
       <c r="I148" s="30">
-        <f>'uap2016'!X153</f>
-        <v>12.685425436698027</v>
+        <f>'uap2016'!E153/'uap2016'!C153</f>
+        <v>4.0302267002518893E-4</v>
       </c>
     </row>
     <row r="149" spans="1:9">
@@ -7929,8 +7929,8 @@
         <v>42.519243708799998</v>
       </c>
       <c r="I149" s="30">
-        <f>'uap2016'!X154</f>
-        <v>8.3845287210783983</v>
+        <f>'uap2016'!E154/'uap2016'!C154</f>
+        <v>3.7679989234288792E-3</v>
       </c>
     </row>
     <row r="150" spans="1:9">
@@ -7967,8 +7967,8 @@
         <v>40.898291814899999</v>
       </c>
       <c r="I150" s="30">
-        <f>'uap2016'!X155</f>
-        <v>10.134422129007019</v>
+        <f>'uap2016'!E155/'uap2016'!C155</f>
+        <v>9.8220640569395019E-3</v>
       </c>
     </row>
     <row r="151" spans="1:9">
@@ -8005,8 +8005,8 @@
         <v>41.497706154500001</v>
       </c>
       <c r="I151" s="30">
-        <f>'uap2016'!X156</f>
-        <v>8.7936699505454836</v>
+        <f>'uap2016'!E156/'uap2016'!C156</f>
+        <v>6.5316278527273435E-3</v>
       </c>
     </row>
     <row r="152" spans="1:9">
@@ -8043,8 +8043,8 @@
         <v>40.3698342637</v>
       </c>
       <c r="I152" s="30">
-        <f>'uap2016'!X157</f>
-        <v>10.598454677911844</v>
+        <f>'uap2016'!E157/'uap2016'!C157</f>
+        <v>5.9716993379202912E-3</v>
       </c>
     </row>
     <row r="153" spans="1:9">
@@ -8081,8 +8081,8 @@
         <v>40.355632654300003</v>
       </c>
       <c r="I153" s="30">
-        <f>'uap2016'!X158</f>
-        <v>10.647211665814998</v>
+        <f>'uap2016'!E158/'uap2016'!C158</f>
+        <v>1.1713074163034132E-2</v>
       </c>
     </row>
     <row r="154" spans="1:9">
@@ -8119,8 +8119,8 @@
         <v>41.510085614200001</v>
       </c>
       <c r="I154" s="30">
-        <f>'uap2016'!X159</f>
-        <v>8.3718568667537969</v>
+        <f>'uap2016'!E159/'uap2016'!C159</f>
+        <v>6.8750810740692697E-3</v>
       </c>
     </row>
     <row r="155" spans="1:9">
@@ -8157,8 +8157,8 @@
         <v>43.310633839700003</v>
       </c>
       <c r="I155" s="30">
-        <f>'uap2016'!X160</f>
-        <v>8.6987493594902467</v>
+        <f>'uap2016'!E160/'uap2016'!C160</f>
+        <v>-3.352540597171294E-3</v>
       </c>
     </row>
     <row r="156" spans="1:9">
@@ -8195,8 +8195,8 @@
         <v>42.033694795300001</v>
       </c>
       <c r="I156" s="30">
-        <f>'uap2016'!X161</f>
-        <v>11.972955763044924</v>
+        <f>'uap2016'!E161/'uap2016'!C161</f>
+        <v>3.8453404087596852E-5</v>
       </c>
     </row>
     <row r="157" spans="1:9">
@@ -8233,8 +8233,8 @@
         <v>41.7708369793</v>
       </c>
       <c r="I157" s="30">
-        <f>'uap2016'!X162</f>
-        <v>8.4247359849257304</v>
+        <f>'uap2016'!E162/'uap2016'!C162</f>
+        <v>8.9691984599229958E-4</v>
       </c>
     </row>
     <row r="158" spans="1:9">
@@ -8271,8 +8271,8 @@
         <v>40.204857509</v>
       </c>
       <c r="I158" s="30">
-        <f>'uap2016'!X163</f>
-        <v>11.88485000577071</v>
+        <f>'uap2016'!E163/'uap2016'!C163</f>
+        <v>9.6417892231647033E-3</v>
       </c>
     </row>
     <row r="159" spans="1:9">
@@ -8309,8 +8309,8 @@
         <v>41.847559380200003</v>
       </c>
       <c r="I159" s="30">
-        <f>'uap2016'!X164</f>
-        <v>12.210912356781311</v>
+        <f>'uap2016'!E164/'uap2016'!C164</f>
+        <v>-2.8490856760764022E-3</v>
       </c>
     </row>
     <row r="160" spans="1:9">
@@ -8347,8 +8347,8 @@
         <v>43.0541751162</v>
       </c>
       <c r="I160" s="30">
-        <f>'uap2016'!X165</f>
-        <v>6.4026203272377709</v>
+        <f>'uap2016'!E165/'uap2016'!C165</f>
+        <v>-5.287881510383243E-3</v>
       </c>
     </row>
     <row r="161" spans="1:9">
@@ -8385,8 +8385,8 @@
         <v>43.5012088525</v>
       </c>
       <c r="I161" s="30">
-        <f>'uap2016'!X166</f>
-        <v>8.2650628605058944</v>
+        <f>'uap2016'!E166/'uap2016'!C166</f>
+        <v>-8.3689789845638836E-4</v>
       </c>
     </row>
     <row r="162" spans="1:9">
@@ -8423,8 +8423,8 @@
         <v>42.060516653599997</v>
       </c>
       <c r="I162" s="30">
-        <f>'uap2016'!X167</f>
-        <v>12.090375353032282</v>
+        <f>'uap2016'!E167/'uap2016'!C167</f>
+        <v>-3.5405192761605035E-3</v>
       </c>
     </row>
     <row r="163" spans="1:9">
@@ -8461,8 +8461,8 @@
         <v>42.3206272364</v>
       </c>
       <c r="I163" s="30">
-        <f>'uap2016'!X168</f>
-        <v>8.0362111179683993</v>
+        <f>'uap2016'!E168/'uap2016'!C168</f>
+        <v>-1.1366028204588508E-3</v>
       </c>
     </row>
     <row r="164" spans="1:9">
@@ -8499,8 +8499,8 @@
         <v>42.5033324228</v>
       </c>
       <c r="I164" s="30">
-        <f>'uap2016'!X169</f>
-        <v>8.9282786936163436</v>
+        <f>'uap2016'!E169/'uap2016'!C169</f>
+        <v>-4.75279978148047E-3</v>
       </c>
     </row>
     <row r="165" spans="1:9">
@@ -8537,8 +8537,8 @@
         <v>41.823443297300003</v>
       </c>
       <c r="I165" s="30">
-        <f>'uap2016'!X170</f>
-        <v>20.062938410977637</v>
+        <f>'uap2016'!E170/'uap2016'!C170</f>
+        <v>6.4181321401720064E-4</v>
       </c>
     </row>
     <row r="166" spans="1:9">
@@ -8575,8 +8575,8 @@
         <v>42.354596287900002</v>
       </c>
       <c r="I166" s="30">
-        <f>'uap2016'!X171</f>
-        <v>10.653007798491986</v>
+        <f>'uap2016'!E171/'uap2016'!C171</f>
+        <v>1.2550636205014133E-3</v>
       </c>
     </row>
     <row r="167" spans="1:9">
@@ -8613,8 +8613,8 @@
         <v>43.365652912100003</v>
       </c>
       <c r="I167" s="30">
-        <f>'uap2016'!X172</f>
-        <v>14.066144983172943</v>
+        <f>'uap2016'!E172/'uap2016'!C172</f>
+        <v>-1.3902216973007554E-3</v>
       </c>
     </row>
     <row r="168" spans="1:9">
@@ -8651,8 +8651,8 @@
         <v>41.760552888600003</v>
       </c>
       <c r="I168" s="30">
-        <f>'uap2016'!X173</f>
-        <v>9.5338350211742675</v>
+        <f>'uap2016'!E173/'uap2016'!C173</f>
+        <v>-4.138387684158252E-4</v>
       </c>
     </row>
     <row r="169" spans="1:9">
@@ -8689,8 +8689,8 @@
         <v>42.844484772000001</v>
       </c>
       <c r="I169" s="30">
-        <f>'uap2016'!X174</f>
-        <v>7.3604015442295747</v>
+        <f>'uap2016'!E174/'uap2016'!C174</f>
+        <v>-2.0801354239889823E-3</v>
       </c>
     </row>
     <row r="170" spans="1:9">
@@ -8727,8 +8727,8 @@
         <v>42.374254694299999</v>
       </c>
       <c r="I170" s="30">
-        <f>'uap2016'!X175</f>
-        <v>8.9561763018208342</v>
+        <f>'uap2016'!E175/'uap2016'!C175</f>
+        <v>-2.6697517130906826E-3</v>
       </c>
     </row>
     <row r="171" spans="1:9">
@@ -8765,8 +8765,8 @@
         <v>42.1649537204</v>
       </c>
       <c r="I171" s="30">
-        <f>'uap2016'!X176</f>
-        <v>8.7905037709539737</v>
+        <f>'uap2016'!E176/'uap2016'!C176</f>
+        <v>-5.4093040028849624E-3</v>
       </c>
     </row>
     <row r="172" spans="1:9">
@@ -8803,8 +8803,8 @@
         <v>43.367915993499999</v>
       </c>
       <c r="I172" s="30">
-        <f>'uap2016'!X177</f>
-        <v>8.3162598999470401</v>
+        <f>'uap2016'!E177/'uap2016'!C177</f>
+        <v>-3.2310177705977385E-3</v>
       </c>
     </row>
     <row r="173" spans="1:9">
@@ -8841,8 +8841,8 @@
         <v>42.489917378500003</v>
       </c>
       <c r="I173" s="30">
-        <f>'uap2016'!X178</f>
-        <v>12.211238342961959</v>
+        <f>'uap2016'!E178/'uap2016'!C178</f>
+        <v>3.594267842972506E-3</v>
       </c>
     </row>
     <row r="174" spans="1:9">
@@ -8879,8 +8879,8 @@
         <v>42.858311276999999</v>
       </c>
       <c r="I174" s="30">
-        <f>'uap2016'!X179</f>
-        <v>10.741030208861838</v>
+        <f>'uap2016'!E179/'uap2016'!C179</f>
+        <v>-1.8946789893116965E-3</v>
       </c>
     </row>
     <row r="175" spans="1:9">
@@ -8917,8 +8917,8 @@
         <v>43.024237270100002</v>
       </c>
       <c r="I175" s="30">
-        <f>'uap2016'!X180</f>
-        <v>9.0204743713248945</v>
+        <f>'uap2016'!E180/'uap2016'!C180</f>
+        <v>-9.0358243860954603E-4</v>
       </c>
     </row>
     <row r="176" spans="1:9">
@@ -8955,8 +8955,8 @@
         <v>43.017430872600002</v>
       </c>
       <c r="I176" s="30">
-        <f>'uap2016'!X181</f>
-        <v>17.67326647290394</v>
+        <f>'uap2016'!E181/'uap2016'!C181</f>
+        <v>-5.8151368010932463E-4</v>
       </c>
     </row>
     <row r="177" spans="1:9">
@@ -8993,8 +8993,8 @@
         <v>42.822785170000003</v>
       </c>
       <c r="I177" s="30">
-        <f>'uap2016'!X182</f>
-        <v>9.5285853695676526</v>
+        <f>'uap2016'!E182/'uap2016'!C182</f>
+        <v>-9.9510974638917322E-4</v>
       </c>
     </row>
     <row r="178" spans="1:9">
@@ -9031,8 +9031,8 @@
         <v>42.829466872399998</v>
       </c>
       <c r="I178" s="30">
-        <f>'uap2016'!X183</f>
-        <v>10.605646993461836</v>
+        <f>'uap2016'!E183/'uap2016'!C183</f>
+        <v>-1.3652862106092729E-3</v>
       </c>
     </row>
     <row r="179" spans="1:9">
@@ -9069,8 +9069,8 @@
         <v>42.937127118200003</v>
       </c>
       <c r="I179" s="30">
-        <f>'uap2016'!X184</f>
-        <v>9.7499506440430768</v>
+        <f>'uap2016'!E184/'uap2016'!C184</f>
+        <v>-1.0483578903227036E-3</v>
       </c>
     </row>
     <row r="180" spans="1:9">
@@ -9107,8 +9107,8 @@
         <v>41.410819531100003</v>
       </c>
       <c r="I180" s="30">
-        <f>'uap2016'!X185</f>
-        <v>8.3128880004317764</v>
+        <f>'uap2016'!E185/'uap2016'!C185</f>
+        <v>-4.00086040008604E-3</v>
       </c>
     </row>
     <row r="181" spans="1:9">
@@ -9145,8 +9145,8 @@
         <v>41.979495952199997</v>
       </c>
       <c r="I181" s="30">
-        <f>'uap2016'!X186</f>
-        <v>12.248484565131577</v>
+        <f>'uap2016'!E186/'uap2016'!C186</f>
+        <v>-1.4938319198149576E-3</v>
       </c>
     </row>
     <row r="182" spans="1:9">
@@ -9183,8 +9183,8 @@
         <v>41.214412600700001</v>
       </c>
       <c r="I182" s="30">
-        <f>'uap2016'!X187</f>
-        <v>10.24354224658005</v>
+        <f>'uap2016'!E187/'uap2016'!C187</f>
+        <v>2.1909047844623402E-3</v>
       </c>
     </row>
     <row r="183" spans="1:9">
@@ -9221,8 +9221,8 @@
         <v>42.247909743400001</v>
       </c>
       <c r="I183" s="30">
-        <f>'uap2016'!X188</f>
-        <v>8.7033960884200301</v>
+        <f>'uap2016'!E188/'uap2016'!C188</f>
+        <v>-3.4142122274320574E-3</v>
       </c>
     </row>
     <row r="184" spans="1:9">
@@ -9259,8 +9259,8 @@
         <v>43.1924527161</v>
       </c>
       <c r="I184" s="30">
-        <f>'uap2016'!X189</f>
-        <v>11.707666407847514</v>
+        <f>'uap2016'!E189/'uap2016'!C189</f>
+        <v>5.0409323708513131E-4</v>
       </c>
     </row>
     <row r="185" spans="1:9">
@@ -9297,8 +9297,8 @@
         <v>41.7513548286</v>
       </c>
       <c r="I185" s="30">
-        <f>'uap2016'!X190</f>
-        <v>12.151698494510949</v>
+        <f>'uap2016'!E190/'uap2016'!C190</f>
+        <v>-2.4172482357986665E-3</v>
       </c>
     </row>
     <row r="186" spans="1:9">
@@ -9335,8 +9335,8 @@
         <v>42.496599146800001</v>
       </c>
       <c r="I186" s="30">
-        <f>'uap2016'!X191</f>
-        <v>23.468078785642032</v>
+        <f>'uap2016'!E191/'uap2016'!C191</f>
+        <v>-3.4605172876704155E-3</v>
       </c>
     </row>
     <row r="187" spans="1:9">
@@ -9373,8 +9373,8 @@
         <v>41.942065661599997</v>
       </c>
       <c r="I187" s="30">
-        <f>'uap2016'!X192</f>
-        <v>7.0224399720182502</v>
+        <f>'uap2016'!E192/'uap2016'!C192</f>
+        <v>-5.2507646087639054E-3</v>
       </c>
     </row>
     <row r="188" spans="1:9">
@@ -9411,8 +9411,8 @@
         <v>41.722517627999999</v>
       </c>
       <c r="I188" s="30">
-        <f>'uap2016'!X193</f>
-        <v>20.483593155048194</v>
+        <f>'uap2016'!E193/'uap2016'!C193</f>
+        <v>-4.0457750549069468E-3</v>
       </c>
     </row>
     <row r="189" spans="1:9">
@@ -9449,8 +9449,8 @@
         <v>41.894397441199999</v>
       </c>
       <c r="I189" s="30">
-        <f>'uap2016'!X194</f>
-        <v>9.7552926172060612</v>
+        <f>'uap2016'!E194/'uap2016'!C194</f>
+        <v>5.1588939331407343E-3</v>
       </c>
     </row>
     <row r="190" spans="1:9">
@@ -9487,8 +9487,8 @@
         <v>41.806405936300003</v>
       </c>
       <c r="I190" s="30">
-        <f>'uap2016'!X195</f>
-        <v>12.132177559391769</v>
+        <f>'uap2016'!E195/'uap2016'!C195</f>
+        <v>1.7744479495268139E-3</v>
       </c>
     </row>
     <row r="191" spans="1:9">
@@ -9525,8 +9525,8 @@
         <v>42.5452310318</v>
       </c>
       <c r="I191" s="30">
-        <f>'uap2016'!X196</f>
-        <v>6.0256874295424323</v>
+        <f>'uap2016'!E196/'uap2016'!C196</f>
+        <v>6.5834925021335394E-3</v>
       </c>
     </row>
     <row r="192" spans="1:9">
@@ -9563,8 +9563,8 @@
         <v>43.256813274999999</v>
       </c>
       <c r="I192" s="30">
-        <f>'uap2016'!X197</f>
-        <v>25.382013081969308</v>
+        <f>'uap2016'!E197/'uap2016'!C197</f>
+        <v>-6.9856556682152664E-3</v>
       </c>
     </row>
     <row r="193" spans="1:9">
@@ -9601,8 +9601,8 @@
         <v>42.143892084000001</v>
       </c>
       <c r="I193" s="30">
-        <f>'uap2016'!X198</f>
-        <v>11.684330221593168</v>
+        <f>'uap2016'!E198/'uap2016'!C198</f>
+        <v>3.1594796731913215E-3</v>
       </c>
     </row>
     <row r="194" spans="1:9">
@@ -9639,8 +9639,8 @@
         <v>40.732097242999998</v>
       </c>
       <c r="I194" s="30">
-        <f>'uap2016'!X199</f>
-        <v>7.3269243258303609</v>
+        <f>'uap2016'!E199/'uap2016'!C199</f>
+        <v>6.1657711618074513E-4</v>
       </c>
     </row>
     <row r="195" spans="1:9">
@@ -9677,8 +9677,8 @@
         <v>43.3877831629</v>
       </c>
       <c r="I195" s="30">
-        <f>'uap2016'!X200</f>
-        <v>36.500156072408693</v>
+        <f>'uap2016'!E200/'uap2016'!C200</f>
+        <v>-7.459852018414136E-3</v>
       </c>
     </row>
     <row r="196" spans="1:9">
@@ -9715,8 +9715,8 @@
         <v>41.672507132900002</v>
       </c>
       <c r="I196" s="30">
-        <f>'uap2016'!X201</f>
-        <v>18.38199765244233</v>
+        <f>'uap2016'!E201/'uap2016'!C201</f>
+        <v>-3.5115955812422268E-3</v>
       </c>
     </row>
     <row r="197" spans="1:9">
@@ -9753,8 +9753,8 @@
         <v>40.832032352100001</v>
       </c>
       <c r="I197" s="30">
-        <f>'uap2016'!X202</f>
-        <v>10.375184709933739</v>
+        <f>'uap2016'!E202/'uap2016'!C202</f>
+        <v>1.8809367064798269E-4</v>
       </c>
     </row>
     <row r="198" spans="1:9">
@@ -9791,8 +9791,8 @@
         <v>42.746391828900002</v>
       </c>
       <c r="I198" s="30">
-        <f>'uap2016'!X203</f>
-        <v>7.670700655418095</v>
+        <f>'uap2016'!E203/'uap2016'!C203</f>
+        <v>-4.2681272049934623E-3</v>
       </c>
     </row>
     <row r="199" spans="1:9">
@@ -9829,8 +9829,8 @@
         <v>41.464099189899997</v>
       </c>
       <c r="I199" s="30">
-        <f>'uap2016'!X204</f>
-        <v>10.454594132157084</v>
+        <f>'uap2016'!E204/'uap2016'!C204</f>
+        <v>7.1966114241065924E-4</v>
       </c>
     </row>
     <row r="200" spans="1:9">
@@ -9867,8 +9867,8 @@
         <v>41.552042430999997</v>
       </c>
       <c r="I200" s="30">
-        <f>'uap2016'!X205</f>
-        <v>7.5333031008109677</v>
+        <f>'uap2016'!E205/'uap2016'!C205</f>
+        <v>-2.3442536482447401E-3</v>
       </c>
     </row>
     <row r="201" spans="1:9">
@@ -9905,8 +9905,8 @@
         <v>42.091393183999998</v>
       </c>
       <c r="I201" s="30">
-        <f>'uap2016'!X206</f>
-        <v>9.0948395800716568</v>
+        <f>'uap2016'!E206/'uap2016'!C206</f>
+        <v>-2.8400126222783212E-3</v>
       </c>
     </row>
     <row r="202" spans="1:9">
@@ -9943,8 +9943,8 @@
         <v>41.634139856399997</v>
       </c>
       <c r="I202" s="30">
-        <f>'uap2016'!X207</f>
-        <v>35.292834762907042</v>
+        <f>'uap2016'!E207/'uap2016'!C207</f>
+        <v>-5.8495081095453335E-3</v>
       </c>
     </row>
     <row r="203" spans="1:9">
@@ -9981,8 +9981,8 @@
         <v>42.373707738699999</v>
       </c>
       <c r="I203" s="30">
-        <f>'uap2016'!X208</f>
-        <v>33.721795561814673</v>
+        <f>'uap2016'!E208/'uap2016'!C208</f>
+        <v>-1.456112581307348E-3</v>
       </c>
     </row>
     <row r="204" spans="1:9">
@@ -10019,8 +10019,8 @@
         <v>43.308012820499997</v>
       </c>
       <c r="I204" s="30">
-        <f>'uap2016'!X209</f>
-        <v>5.3891619891565785</v>
+        <f>'uap2016'!E209/'uap2016'!C209</f>
+        <v>-4.1666666666666666E-3</v>
       </c>
     </row>
     <row r="205" spans="1:9">
@@ -10057,8 +10057,8 @@
         <v>42.375902139600001</v>
       </c>
       <c r="I205" s="30">
-        <f>'uap2016'!X210</f>
-        <v>11.495850952822332</v>
+        <f>'uap2016'!E210/'uap2016'!C210</f>
+        <v>-5.4813542599258193E-5</v>
       </c>
     </row>
     <row r="206" spans="1:9">
@@ -10095,8 +10095,8 @@
         <v>42.237269812900003</v>
       </c>
       <c r="I206" s="30">
-        <f>'uap2016'!X211</f>
-        <v>6.9046440115312855</v>
+        <f>'uap2016'!E211/'uap2016'!C211</f>
+        <v>-1.4910907328710953E-4</v>
       </c>
     </row>
     <row r="207" spans="1:9">
@@ -10133,8 +10133,8 @@
         <v>41.95363558837586</v>
       </c>
       <c r="I207" s="30">
-        <f>'uap2016'!X212</f>
-        <v>47.483322823018526</v>
+        <f>'uap2016'!E212/'uap2016'!C212</f>
+        <v>8.021035401575E-3</v>
       </c>
     </row>
   </sheetData>
@@ -10148,10 +10148,10 @@
   <dimension ref="A1:AS212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E93" sqref="E7:E212"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>